<commit_message>
editing house and agent to add primary key, official listing table added
</commit_message>
<xml_diff>
--- a/Excel Files for Table/Listing.xlsx
+++ b/Excel Files for Table/Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anime\FinalProject\Excel Files for Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDCFF55-F38E-401F-856E-14793E27622B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C712C-32D0-48E0-B142-DF24841069BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C65578F-E978-4909-95A3-1344B22CB78C}"/>
   </bookViews>
@@ -50,12 +50,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>sample description 2</t>
-  </si>
-  <si>
-    <t>sample description 3</t>
-  </si>
-  <si>
     <t>date_listed</t>
   </si>
   <si>
@@ -74,6 +68,13 @@
 The master bedroom has new hardwood floors, is also located on the main floor and has a large walk-in closet with custom shelving. 
 The 1st fl bedroom includes a built-in shelving unit, plenty of storage, and a private full bathroom. Each level has its own luxurious, full bathroom with granite vanities. 
 Additional features include CENTRAL AIR, lots of storage, and side garden! The garage has a built-in storage unit and second refrigerator for extra storage. </t>
+  </si>
+  <si>
+    <t>2 Bedroom 1 Bath complete remodel. Updated kitchen: center island, New cabinets, New appliances, Granite counter tops. Great views of the backyard from the kitchen and breakfast room windows! Remodel and new appliances 2023. Open concept. Vaulted Living area. Tall baseboards through out, and New Luxury Vinyl plank flooring. New windows to help keep your utility bills down, hot water heater. HVAC recently services and new AC outside unit (condenser) installed. Large backyard. Close to Six Flags, Hurricane Harbor, Globe Life Field, AT&amp;T stadium, and more! Great Location!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome home to this brand new bi-level condo on Aldine! This condo is perfectly positioned to access all of the great restaurants and retail shops in the area! Enter unit A to a stunning open-concept living area that leads into a wrap-around kitchen equipped with quartz counters, stainless steel appliances and marble backsplash. Bedrooms on both floors offer tons of space and have direct access to a private bath.
+</t>
   </si>
 </sst>
 </file>
@@ -135,6 +136,127 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07581AF5-8BC5-E27F-A7C2-7D64AAD93E4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="640080" y="7010400"/>
+          <a:ext cx="7658100" cy="2727960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Links for</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> descriptions</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>4402 Driftwood Dr, Philadelphia, PA 19129 | Zillow</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>407 W Oxford St, Philadelphia, PA 19122, USA - 3 unit Rentals | Zumper</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>2501 Oak Hill Drive, Arlington, TX 76006, USA | 2 bed duplex for rent #90051616 | Rentberry</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D5E49D-3222-49A5-B9C9-94F9E995A743}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,13 +587,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
@@ -485,7 +607,7 @@
         <v>1234</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3">
         <v>45175</v>
@@ -497,7 +619,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3548</v>
       </c>
@@ -507,8 +629,8 @@
       <c r="C3" s="1">
         <v>5678</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="3">
         <v>45223</v>
@@ -520,7 +642,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1759</v>
       </c>
@@ -530,8 +652,8 @@
       <c r="C4" s="1">
         <v>9102</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="3">
         <v>45244</v>
@@ -545,5 +667,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>